<commit_message>
se agrega idubicacionorigen y idubicaciondestino a tabla de movimientos de mercancia de pedidos especiales
</commit_message>
<xml_diff>
--- a/Analisis/SPRINTs/Back log SPRINT 11.xlsx
+++ b/Analisis/SPRINTs/Back log SPRINT 11.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Back log" sheetId="1" r:id="rId1"/>
     <sheet name="Cuentas X Cobrar" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -646,10 +646,13 @@
   <dimension ref="A1:O113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="B12" sqref="B12:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="22.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -732,16 +735,16 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
       <c r="J4" s="9">
         <v>44512</v>
       </c>
@@ -1076,7 +1079,7 @@
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
     </row>
-    <row r="18" spans="1:15" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1126,7 +1129,7 @@
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
     </row>
-    <row r="20" spans="1:15" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
se agrego dropdown de acciones en vista de entregar productos
</commit_message>
<xml_diff>
--- a/Analisis/SPRINTs/Back log SPRINT 11.xlsx
+++ b/Analisis/SPRINTs/Back log SPRINT 11.xlsx
@@ -646,7 +646,7 @@
   <dimension ref="A1:O113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:I12"/>
+      <selection activeCell="B5" sqref="B5:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,16 +760,16 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
       <c r="J5" s="9">
         <v>44512</v>
       </c>
@@ -3194,6 +3194,7 @@
     <mergeCell ref="N16:O16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>